<commit_message>
another commit new in d-base
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,50 +424,50 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>LTC3404MPMS8#PBF</t>
+          <t>OP193FSZ</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>584-LTC3404MPMS8#PBF</t>
+          <t>584-OP193FSZ</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Импульсные регуляторы напряжения Military Plastic: 600mA, 1.4MHz Synch Buck Reg</t>
+          <t>Прецизионные усилители MICROPOWER RAIL TO RAIL</t>
         </is>
       </c>
       <c r="D1" t="n">
-        <v>0.00023375</v>
+        <v>0.00054</v>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>https://www.mouser.com/images/adi/images/ITP_ADI_MSOP_05-08-1660_t.jpg</t>
+          <t>https://www.mouser.com/images/adi/images/ITP_ADI_SOIC-8_R-8_t.jpg</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>https://ru.mouser.com/ProductDetail/Analog-Devices/LTC3404MPMS8PBF?qs=hVkxg5c3xu%252BYfsSnKWgFNA%3D%3D</t>
+          <t>https://ru.mouser.com/ProductDetail/Analog-Devices/OP193FSZ?qs=WIvQP4zGangdcMDFxf52bQ%3D%3D</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>{'Категория продукта': 'Импульсные регуляторы напряжения', 'Вид монтажа': 'SMD/SMT', 'Упаковка / блок': 'MSOP-8', 'Топология': 'Buck', 'Выходное напряжение': '800 mV to 6 V', 'Выходной ток': '600 mA', 'Количество выходов': '1 Output', 'Входное напряжение (макс.)': '6 V', 'Входное напряжение МИН.': '2.65 V', 'Ток покоя': '10 uA', 'Частота переключений': '1.4 MHz', 'Минимальная рабочая температура': '- 55 C', 'Максимальная рабочая температура': '+ 125 C', 'Серия': 'LTC3404', 'Входное напряжение': '3.6 V', 'Тип': 'Monolithic Synchronous Step-Down Buck Regulator', 'Отключение': 'Shutdown', 'Средства разработки': 'DC413A', 'Рабочий ток источника питания': '0.01 mA'}</t>
+          <t>{'Категория продукта': 'Прецизионные усилители', 'Серия': 'OP193', 'Количество каналов': '1 Channel', 'GBP - Произведение коэффициента усиления на ширину полосы пропускания (fT)': '35 kHz', 'SR - скорость нарастания выходного напряжения': '12 V/us', 'CMRR - Коэффициент подавления синфазного сигнала': '116 dB', 'Выходной ток на канал': '25 mA', 'Ib - Входной ток смещения': '20 nA', 'Vos - Входное напряжение смещения нуля': '150 uV', 'en - Интенсивность шума входного напряжения': '65 nV/sqrt Hz', 'Напряжение питания - макс.': '36 V, +/- 18 V', 'Напряжение питания - мин.': '1.7 V, +/- 1 V', 'Рабочий ток источника питания': '30 uA', 'Минимальная рабочая температура': '- 40 C', 'Максимальная рабочая температура': '+ 125 C', 'Отключение': 'No Shutdown', 'Вид монтажа': 'SMD/SMT', 'Упаковка / блок': 'SOIC-8', 'Высота': '1.5 mm (Max)', 'Длина': '5 mm (Max)', 'Продукт': 'Precision Amplifiers', 'Тип': 'Precision', 'Ширина': '4 mm (Max)', 'Диапазон входного напряжения - макс.': '13.5 V', 'Средства разработки': 'EVAL-CN0319-EB1Z', 'Напряжение сдвоенного питания': '+/- 0.85 V to +/- 18 V', 'Максимальное напряжение сдвоенного питания': '+/- 18 V', 'Минимальное напряжение сдвоенного питания': '+/- 1 V', 'PSRR - Коэффициент подавления помех по питанию': '120 dB', 'Усиление по напряжению, дБ': '106.02 dB'}</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>https://ru.mouser.com/datasheet/2/609/3404fb-1266354.pdf</t>
+          <t>https://ru.mouser.com/datasheet/2/609/OP193_293-1504363.pdf</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Интегральные монолитные схемы — Импульсные регуляторы напряжения. Выходное напряжение 800 мВ ... 6 В, Выходной ток 600 мА, Входное напряжение от 2.65 В до 6 В, Частота переключений 1.4 МГц, Рабочий ток источника питания 0.01 мА, корпус MSOP-8, рабочие температуры от -40 до 85°С, предназначены для монтажа на печатную плату радиоэлектронного оборудования общепромышленного назначения.</t>
+          <t xml:space="preserve"> Интегральные монолитные схемы — Прецизионные усилители. Количество каналов 1, Произведение коэффициента усиления на ширину полосы пропускания  35 кГц, Коэффициент подавления синфазного сигнала 116 дБ, Выходной ток на канал 25 мА, Входной ток смещения 20 нA, Рабочий ток источника питания 30 мкА, рабочая температура от - 40 C до + 125 C, Вид монтажа: на поверхность печатной платы, тип корпуса SOIC-8, Диапазон входного напряжения - макс. 13.5 В, Напряжение сдвоенного питания +/- 0.85 В...+/- 18 В, Коэффициент подавления помех по питанию 120 дБ, Усиление по напряжению 106.02 дБ, предназначены для монтажа в радиоэлектронное оборудование общепромышленного назначения.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Категория продукта Импульсные регуляторы напряжения</t>
+          <t>Категория продукта Прецизионные усилители</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
@@ -477,198 +477,138 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>LTC3404MPMS8#PBF</t>
+          <t>OP193FSZ</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MAX8640ZEXT12+</t>
+          <t>REF192FSZ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>700-MAX8640ZEXT12TNR</t>
+          <t>584-REF192FSZ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Импульсные регуляторы напряжения 500mA 4/2MHz Synch Step-Down DC/DC Conv</t>
+          <t>Источники опорного напряжения MICROPOWER VOLTAGE REF</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2.8e-05</v>
+        <v>0.00054</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://www.mouser.com/images/mouserelectronics/images/SC_70_6_t.jpg</t>
+          <t>https://www.mouser.com/images/adi/images/ITP_ADI_SOIC-8_R-8_t.jpg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://ru.mouser.com/ProductDetail/Maxim-Integrated/MAX8640ZEXT12-T?qs=7JzFWu92cmgYRHsc4BTGuQ%3D%3D</t>
+          <t>https://ru.mouser.com/ProductDetail/Analog-Devices/REF192FSZ?qs=WIvQP4zGang37SU8A%2F%2Fv2g%3D%3D</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>{'Категория продукта': 'Импульсные регуляторы напряжения', 'Вид монтажа': 'SMD/SMT', 'Упаковка / блок': 'SC70-6', 'Топология': 'Buck', 'Выходное напряжение': '800 mV to 2.5 V', 'Выходной ток': '500 mA', 'Входное напряжение (макс.)': '5.5 V', 'Входное напряжение МИН.': '2.7 V', 'Частота переключений': '4 MHz', 'Серия': 'MAX8640Z', 'Тип': 'Voltage Converter'}</t>
+          <t>{'Категория продукта': 'Источники опорного напряжения', 'Вид монтажа': 'SMD/SMT', 'Упаковка / блок': 'SOIC-8', 'Тип ссылки': 'Series Precision References', 'Выходное напряжение': '2.5 V', 'Исходная точность': '0.08 %', 'Температурный коэффициент': '10 PPM/C', 'Серия VREF - входное напряжение - макс.': '18 V', 'Ток через шунт - макс.': '30 mA', 'Минимальная рабочая температура': '- 40 C', 'Максимальная рабочая температура': '+ 85 C', 'Серия': 'REF192', 'Точность': '15 PPM/mA', 'Высота': '1.5 mm (Max)', 'Входное напряжение': '18 V', 'Длина': '5 mm (Max)', 'Выходной ток': '30 mA', 'Ширина': '4 mm (Max)', 'Топология': 'Series References', 'Нестабильность выходной нагрузки': '15 PPM/mA'}</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://ru.mouser.com/datasheet/2/256/MAX8640Z-1514322.pdf</t>
+          <t>https://ru.mouser.com/datasheet/2/609/REF19xSeries-879583.pdf</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Интегральные монолитные схемы — Импульсные регуляторы напряжения. Выходное напряжение 800 мВ ... 2.5 В, Выходной ток 500 мА, Входное напряжение от 2.7 В до 5.5 В, Частота переключений 4 МГц, корпус SC70-6, рабочие температуры от -40 до 85°С, предназначены для монтажа на печатную плату радиоэлектронного оборудования общепромышленного назначения.</t>
+          <t>Интегральные монолитные схемы — схемы эталонного напряжения. Выходное напряжение 2.5 В, Исходная точность 0.08 %, ток через шунт до 30 мА, входное напряжение от 18 В, корпус SOIC-8, рабочие температуры от -40 до 85°С, предназначены для использования в радиоэлектронном оборудовании общепромышленного назначения.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Категория продукта Импульсные регуляторы напряжения</t>
+          <t>Категория продукта Источники опорного напряжения</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Maxim Integrated</t>
+          <t>Analog Devices</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>MAX8640ZEXT12-T</t>
+          <t>REF192FSZ</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LY ETSF-ABCA-46-1</t>
+          <t>MC9S12DG128BCFU</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>841-MC9S12DG128BCF</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>16-битные микроконтроллеры 16 Bit 25MHz</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0009355</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.mouser.com/images/mouserelectronics/images/PQFP_80_Sq_t.jpg</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://ru.mouser.com/ProductDetail/NXP-Semiconductors/MC9S12DG128BCFU?qs=XE3KHhr8I8H9wWGLTTxabA%3D%3D</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>{'Категория продукта': '16-битные микроконтроллеры', 'Вид монтажа': 'SMD/SMT', 'Упаковка / блок': 'PQFP-80', 'Ядро': 'HCS12', 'Размер программной памяти': '128 kB', 'Ширина шины данных': '16 bit', 'Разрешение АЦП': '2 x 10 bit', 'Максимальная тактовая частота': '50 MHz', 'Количество входов/выходов': '59 I/O', 'Размер ОЗУ данных': '8 kB', 'Рабочее напряжение питания': '5 V', 'Минимальная рабочая температура': '- 40 C', 'Максимальная рабочая температура': '+ 85 C', 'Высота': '2.4 mm', 'Длина': '14.1 mm', 'Продукт': 'MCU', 'Тип памяти программ': 'EEPROM', 'Ширина': '14.1 mm', 'Тип ОЗУ данных': 'RAM', 'Размер ПЗУ данных': '2 kB', 'Тип ПЗУ данных': 'EEPROM', 'Тип интерфейса': 'CAN, I2C, SCI, SPI', 'Количество каналов АЦП': '8 Channel, 8 Channel', 'Количество таймеров/счетчиков': '1 Timer', 'Серия процессора': 'HCS12'}</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://ru.mouser.com/datasheet/2/302/NXP_04042019_MC9S12A128BCFU-1551128.pdf</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Интегральные монолитные схемы — 16-битные микроконтроллеры. Вид монтажа на поверхность печатной платы, тип корпуса PQFP-80, Ядро HCS12, Ширина шины данных 16 бит, Максимальная тактовая частота 50 МГц, Количество входов/выходов 59, Рабочее напряжение питания 5 В, рабочая температура от - 40 C до + 85 C, Тип интерфейса CAN, I2C, SCI, SPI. Не содержат функции шифрования и криптографии, предназначены для монтажа на печатную плату радиоэлектронного оборудования общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Категория продукта 16-битные микроконтроллеры</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>NXP Semiconductors</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>MC9S12DG128BCFU</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TAJV687M010RNJV</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>581-TAJV687M010RNJV</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Танталовые конденсаторы - твердые, для поверхностного монтажа 680uF 10V 20% 7361 ESR 400mOhm Low Prof</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.000766282984293</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://www.mouser.com/images/avx/images/TAJ_series_DSL.jpg</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>https://ru.mouser.com/ProductDetail/AVX/TAJV687M010RNJV?qs=AQlKX63v8RuzjrOQF2CwbA%3D%3D</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>{'Категория продукта': 'Танталовые конденсаторы - твердые, для поверхностного монтажа', 'Серия': 'TAJ', 'Ёмкость': '680 uF', 'Номинальное напряжение постоянного тока': '10 VDC', 'Допустимое отклонение': '20 %', 'Эффективное последовательное сопротивление': '400 mOhms', 'Корпус - дюймы': '2924', 'Корпус - мм': '7361', 'Рег. код произв.': 'V Case', 'Минимальная рабочая температура': '- 55 C', 'Максимальная рабочая температура': '+ 125 C', 'Тип выводов': 'SMD/SMT', 'Продукт': 'Tantalum Solid Standard Grade - Other Various'}</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>https://ru.mouser.com/datasheet/2/40/taj-776811.pdf</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Конденсаторы танталовые, постоянной емкости, с номиналом 680 мкФ, рабочее напряжение 10 В постоянного тока, допустимое отклонение 20 %, тип корпуса 2924, монтаж на поверхность печатной платы, рабочие температуры от -40 до 125°С, предназначены для монтажа в радиоэлектронном оборудовании общепромышленного назначения.</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Категория продукта Танталовые конденсаторы - твердые</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>AVX</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>TAJV687M010RNJV</t>
+          <t>K9F1G08U0B-PIB0</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SB3H90E3/54</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>625-SB3H90-E3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Диоды и выпрямители Шоттки 3.0 Amp 90 Volt</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0.0011</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://www.mouser.com/images/vishay/images/do204ac.jpg</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>https://ru.mouser.com/ProductDetail/Vishay-General-Semiconductor/SB3H90-E3-54?qs=u91jd7aysvPU%2FYnn5DDDQg%3D%3D</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>{'Категория продукта': 'Диоды и выпрямители Шоттки', 'Продукт': 'Schottky Diodes', 'Вид монтажа': 'Through Hole', 'Упаковка / блок': 'DO-201AD-2', 'Конфигурация': 'Single', 'Технология': 'Si', 'If - прямой ток': '3 A', 'Vrrm - повторяющееся обратное напряжение': '90 V', 'Vf - прямое напряжение': '800 mV', 'Ifsm - ударный прямой ток': '100 A', 'Ir - обратный ток ': '20 uA', 'Минимальная рабочая температура': '- 55 C', 'Максимальная рабочая температура': '+ 175 C', 'Высота': '5.3 mm', 'Длина': '9.5 mm', 'Тип выводов': 'Axial', 'Тип': 'Schottky Diode', 'Ширина': '5.3 mm'}</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>https://ru.mouser.com/datasheet/2/427/sb3h90-1768379.pdf</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Диоды Шоттки, полупроводниковые. Обратный ток 20 мкА, Прямое напряжение 800 мВ, Прямой ток 3 A,  Тип корпуса DO-201AD-2, монтаж в отверстия печатной платы, рабочая температура от -40 до 85°С. Используются для монтажа в радиоэлектронных устройствах общепромышленного применения.</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Категория продукта Диоды и выпрямители Шоттки</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Vishay General Semiconductor</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>SB3H90-E3/54</t>
-        </is>
-      </c>
-    </row>
-    <row r="6"/>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>